<commit_message>
Update exam data structure and UI with topic names
</commit_message>
<xml_diff>
--- a/exam.xlsx
+++ b/exam.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e.bilolov\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e.bilolov\Desktop\Visual Studio\exam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5A3095-B951-423D-BD50-5CAE8B73203D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C34CAD-51B6-4C9C-B1E1-01E6A02BCB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="240" windowWidth="14340" windowHeight="17265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14415" yWindow="30" windowWidth="14340" windowHeight="17265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="347">
   <si>
     <t>Part 1</t>
   </si>
@@ -312,15 +312,9 @@
     <t>4.  What do you like eating at a restaurant?</t>
   </si>
   <si>
-    <t>Question</t>
-  </si>
-  <si>
     <t>Xarid qilishni yoqtirasanmi?</t>
   </si>
   <si>
-    <t>UZ tarjima:</t>
-  </si>
-  <si>
     <t>Yakshanba kunlari xarid qilasanmi?</t>
   </si>
   <si>
@@ -328,12 +322,6 @@
   </si>
   <si>
     <t>Sening mamlakatingda kiyimlar arzonmi?</t>
-  </si>
-  <si>
-    <t>Answer (EN):</t>
-  </si>
-  <si>
-    <t>Javob (UZ):</t>
   </si>
   <si>
     <t>Yes, I like shopping.
@@ -586,9 +574,6 @@
     <t>Men uyda yashayman.</t>
   </si>
   <si>
-    <t>Sizning uyingizda/qvartirangizda nechta xona bor?</t>
-  </si>
-  <si>
     <t>There are five bedrooms, two living rooms, two bathrooms, one toilet, and one kitchen.</t>
   </si>
   <si>
@@ -652,6 +637,492 @@
   <si>
     <t>Mening uyimda tekin internet va konditsioner bor.
 Chiroyli bog‘imiz ham bor.</t>
+  </si>
+  <si>
+    <t>Siz kafelarga borishni yoqtirasizmi?</t>
+  </si>
+  <si>
+    <t>Yes, I like going to cafés. I go with my friends.</t>
+  </si>
+  <si>
+    <t>Ha, men kafelarga borishni yoqtiraman. Do‘stlarim bilan boraman.</t>
+  </si>
+  <si>
+    <t>Sizning shahringizda qaysi kafelar mashhur?</t>
+  </si>
+  <si>
+    <t>Basri Baba and Zoxid Kabob are popular cafés in my town.</t>
+  </si>
+  <si>
+    <t>Mening shahrimda Basri Baba va Zoxid Kabob mashhur.</t>
+  </si>
+  <si>
+    <t>Siz kafeda qaysi ovqat va ichimliklarni yoqtirasiz?</t>
+  </si>
+  <si>
+    <t>I like Zoxid Kabob. It is very tasty.</t>
+  </si>
+  <si>
+    <t>Men Zoxid kabobni yoqtiraman. U juda mazali.</t>
+  </si>
+  <si>
+    <t>Sizning mamlakatingizda/shahringizda kafelar qimmatmi?</t>
+  </si>
+  <si>
+    <t>No, cafés are not very expensive. The prices are average.</t>
+  </si>
+  <si>
+    <t>Yo‘q, kafelar juda qimmat emas. Narxlari o‘rtacha.</t>
+  </si>
+  <si>
+    <t>Kelajakdagi rejalaringiz qanday?</t>
+  </si>
+  <si>
+    <t>My plans for the future are to learn English and travel around the world.</t>
+  </si>
+  <si>
+    <t>Kelajakdagi rejalarim ingliz tilini o‘rganish va dunyoni kezish.</t>
+  </si>
+  <si>
+    <t>Imtihondan keyin nima qilmoqchisiz?</t>
+  </si>
+  <si>
+    <t>Siz O‘zbekistonda yoki boshqa davlatda o‘qimoqchimisiz?</t>
+  </si>
+  <si>
+    <t>I am going to study for a master’s degree in the USA.</t>
+  </si>
+  <si>
+    <t>Men magistraturani AQShda o‘qimoqchiman.</t>
+  </si>
+  <si>
+    <t>Bu hafta oxirida nima qilmoqchisiz?</t>
+  </si>
+  <si>
+    <t>This weekend, I am going to cook plov for my family.</t>
+  </si>
+  <si>
+    <t>Bu hafta oxirida oilam uchun palov pishirib bermoqchiman.</t>
+  </si>
+  <si>
+    <t>Imtihondan keyin KFCga borib ovqatlanmoqchiman.</t>
+  </si>
+  <si>
+    <t>After the exam, I am going to go to KFC and eat food.</t>
+  </si>
+  <si>
+    <t>Sizning yaxshi qo‘shnilaringiz bormi? Ular kimlar?</t>
+  </si>
+  <si>
+    <t>Yes, I have good neighbours. They are kind and friendly people.</t>
+  </si>
+  <si>
+    <t>Ha, mening yaxshi qo‘shnilarim bor. Ular mehribon va inoq insonlar.</t>
+  </si>
+  <si>
+    <t>Ularning kasbi nima?</t>
+  </si>
+  <si>
+    <t>They are a doctor, a banker, a taxi driver, and a businessman.</t>
+  </si>
+  <si>
+    <t>Ular shifokor, bank xodimi, taksichi va biznesmen.</t>
+  </si>
+  <si>
+    <t>Siz qo‘shnilaringiz bilan tez-tez gaplashasizmi?</t>
+  </si>
+  <si>
+    <t>Yes, I talk to them every day. I see them often.</t>
+  </si>
+  <si>
+    <t>Ha, men ular bilan har kuni gaplashaman. Tez-tez ko‘raman.</t>
+  </si>
+  <si>
+    <t>Siz qo‘shnilaringizga yordam berasizmi?</t>
+  </si>
+  <si>
+    <t>Yes, I help my neighbours. I help them when I can.</t>
+  </si>
+  <si>
+    <t>Ha, men qo‘shnilarimga yordam beraman. Qo‘limdan kelgancha yordam qilaman.</t>
+  </si>
+  <si>
+    <t>Yoningizdagi qo‘shningiz haqida gapirib bering.</t>
+  </si>
+  <si>
+    <t>My next door neighbour is a doctor. He is a very kind person.</t>
+  </si>
+  <si>
+    <t>Mening yonimdagi qo‘shnim shifokor. U juda yaxshi inson.</t>
+  </si>
+  <si>
+    <t>Siz odatda qo‘shningizni qachon uchratasiz?</t>
+  </si>
+  <si>
+    <t>I usually meet my neighbour in the morning and in the evening.</t>
+  </si>
+  <si>
+    <t>Men qo‘shnimni odatda ertalab va kechqurun uchrataman.</t>
+  </si>
+  <si>
+    <t>Qo‘shningizning uy hayvoni bormi?</t>
+  </si>
+  <si>
+    <t>Yes, my neighbour has chickens.</t>
+  </si>
+  <si>
+    <t>Ha, qo‘shnimning tovuqlari bor.</t>
+  </si>
+  <si>
+    <t>Siz qo‘shningizni yoqtirasizmi? Nima uchun?</t>
+  </si>
+  <si>
+    <t>Yes, I like my neighbour because he is kind.</t>
+  </si>
+  <si>
+    <t>Ha, men qo‘shnimni yoqtiraman, chunki u yaxshi inson.</t>
+  </si>
+  <si>
+    <t>Sizning uyingizda/kvartirangizda nechta xona bor?</t>
+  </si>
+  <si>
+    <t>Sizning oilangizda nechta odam bor?</t>
+  </si>
+  <si>
+    <t>There are nine people in my family. We live together.</t>
+  </si>
+  <si>
+    <t>Mening oilamda to‘qqiz kishi bor. Biz birga yashaymiz.</t>
+  </si>
+  <si>
+    <t>Sizning aka-uka yoki opa-singillaringiz bormi? Ularning ismlari qanday?</t>
+  </si>
+  <si>
+    <t>Yes, I have a brother and a younger brother. Their names are Doniyor and Ismoil.</t>
+  </si>
+  <si>
+    <t>Ha, mening akam va ukam bor. Ularning ismlari Doniyor va Ismoil.</t>
+  </si>
+  <si>
+    <t>Ota-onangizning kasbi nima?</t>
+  </si>
+  <si>
+    <t>My mother is a housewife. My father passed away.</t>
+  </si>
+  <si>
+    <t>Onam uy bekasi. Otam olamdan o‘tganlar.</t>
+  </si>
+  <si>
+    <t>Siz oilangiz bilan nima qilishni yoqtirasiz?</t>
+  </si>
+  <si>
+    <t>I like travelling with my family.</t>
+  </si>
+  <si>
+    <t>Men oilam bilan sayohat qilishni yoqtiraman.</t>
+  </si>
+  <si>
+    <t>My Daily Life</t>
+  </si>
+  <si>
+    <t>My House</t>
+  </si>
+  <si>
+    <t>Cafes and My Plans</t>
+  </si>
+  <si>
+    <t>My Neighbours</t>
+  </si>
+  <si>
+    <t>My Family</t>
+  </si>
+  <si>
+    <t>Life</t>
+  </si>
+  <si>
+    <t>Shopping</t>
+  </si>
+  <si>
+    <t>Haftaning qaysi kunini eng yaxshi ko‘rasiz?</t>
+  </si>
+  <si>
+    <t>My favourite day is Sunday because I can rest.</t>
+  </si>
+  <si>
+    <t>Eng sevimli kunim yakshanba, chunki dam olaman.</t>
+  </si>
+  <si>
+    <t>Yakshanba kunlari oilangiz bilan nima qilasiz?</t>
+  </si>
+  <si>
+    <t>We go shopping and cook dinner together.</t>
+  </si>
+  <si>
+    <t>Biz birga xarid qilamiz va kechki ovqatni tayyorlaymiz.</t>
+  </si>
+  <si>
+    <t>Oxirgi safar oilangiz bilan qayerga bordingiz?</t>
+  </si>
+  <si>
+    <t>We went to City Mall to buy clothes.</t>
+  </si>
+  <si>
+    <t>Oxirgi safar kiyim olish uchun City Mallga bordik.</t>
+  </si>
+  <si>
+    <t>Oilangiz bilan vaqtni qanday o‘tkazdingiz?</t>
+  </si>
+  <si>
+    <t>We watched a film and talked together.</t>
+  </si>
+  <si>
+    <t>Biz film ko‘rdik va birga suhbatlashdik.</t>
+  </si>
+  <si>
+    <t>Sizning do‘stlaringiz bormi?</t>
+  </si>
+  <si>
+    <t>Yes, I have many friends.</t>
+  </si>
+  <si>
+    <t>Ha, mening juda ko‘p do‘stlarim bor.</t>
+  </si>
+  <si>
+    <t>Siz do‘stlaringiz bilan tez-tez uchratasizmi?</t>
+  </si>
+  <si>
+    <t>We meet once a week.</t>
+  </si>
+  <si>
+    <t>Biz haftasiga bir marta uchrashamiz.</t>
+  </si>
+  <si>
+    <t>Sizning eng yaqin do‘stingiz kim?</t>
+  </si>
+  <si>
+    <t>My best friend is Anvar. I have known him since childhood.</t>
+  </si>
+  <si>
+    <t>Eng yaqin do‘stim Anvar. Men uni bolaligimizdan taniyman.</t>
+  </si>
+  <si>
+    <t>Sizning do‘stingiz nimani yoqtiradi?</t>
+  </si>
+  <si>
+    <t>He likes travelling.</t>
+  </si>
+  <si>
+    <t>U sayohat qilishni yoqtiradi.</t>
+  </si>
+  <si>
+    <t>Do‘stlaringiz bilan uchrashishni yoqtirasizmi?</t>
+  </si>
+  <si>
+    <t>Yes, I like meeting my friends.</t>
+  </si>
+  <si>
+    <t>Ha, men do‘stlarim bilan uchrashishni yoqtiraman.</t>
+  </si>
+  <si>
+    <t>Ularni oxirgi safar qachon uchratdingiz? Qayerda?</t>
+  </si>
+  <si>
+    <t>We met last Sunday in a café.</t>
+  </si>
+  <si>
+    <t>Biz oxirgi safar o‘tgan yakshanba kuni kafeda uchrashdik.</t>
+  </si>
+  <si>
+    <t>Siz birga nima qildingiz?</t>
+  </si>
+  <si>
+    <t>We ate food and talked together.</t>
+  </si>
+  <si>
+    <t>Biz ovqatlandik va birga suhbatlashdik.</t>
+  </si>
+  <si>
+    <t>Sizga yoqdimi?</t>
+  </si>
+  <si>
+    <t>Yes, I liked it.</t>
+  </si>
+  <si>
+    <t>Ha, menga yoqdi.</t>
+  </si>
+  <si>
+    <t>My friends</t>
+  </si>
+  <si>
+    <t>Siz ishlaysizmi yoki talabasizmi?</t>
+  </si>
+  <si>
+    <t>I work at the Republican Cadastre.</t>
+  </si>
+  <si>
+    <t>Men Respublika kadastrda ishlayman.</t>
+  </si>
+  <si>
+    <t>Sizning orzuingizdagi kasb nima?</t>
+  </si>
+  <si>
+    <t>My dream job is to be a businessman.</t>
+  </si>
+  <si>
+    <t>Orzuimdagi kasb biznesmen bo‘lish.</t>
+  </si>
+  <si>
+    <t>Siz ofisda ishlaysizmi?</t>
+  </si>
+  <si>
+    <t>Yes, I work in an office.</t>
+  </si>
+  <si>
+    <t>Ha, men ofisda ishlayman.</t>
+  </si>
+  <si>
+    <t>Sizning ish joyingiz shifoxonadami?</t>
+  </si>
+  <si>
+    <t>No, I don’t work in a hospital.</t>
+  </si>
+  <si>
+    <t>Yo‘q, men shifoxonada ishlamayman.</t>
+  </si>
+  <si>
+    <t>Siz odatda ishga yoki maktabga qanday borasiz?</t>
+  </si>
+  <si>
+    <t>I have a car. I go to work by car.</t>
+  </si>
+  <si>
+    <t>Menda mashinam bor. Ishga mashinada boraman.</t>
+  </si>
+  <si>
+    <t>Sizning sevimli transport turingiz qaysi?</t>
+  </si>
+  <si>
+    <t>My favorite transport is the metro because it is very fast.</t>
+  </si>
+  <si>
+    <t>Sevimli transportim metro, chunki u juda tez yuradi.</t>
+  </si>
+  <si>
+    <t>I travelled to Samarkand. It is famous for old buildings.</t>
+  </si>
+  <si>
+    <t>Siz qilgan sayohatingiz haqida gapiring.</t>
+  </si>
+  <si>
+    <t>Men Samarqandga sayohat qilganman. U eski binolari bilan mashhur.</t>
+  </si>
+  <si>
+    <t>Odamlar jamoat transportidan qanchalik tez foydalanadi?</t>
+  </si>
+  <si>
+    <t>People often use public transport every day.</t>
+  </si>
+  <si>
+    <t>Odamlar har kuni jamoat transportidan tez-tez foydalanadi.</t>
+  </si>
+  <si>
+    <t>Bugun quyoshli kunmi?</t>
+  </si>
+  <si>
+    <t>Siz yomg‘irli ob-havoni yoqtirasizmi?</t>
+  </si>
+  <si>
+    <t>Yes, I like rainy weather very much.</t>
+  </si>
+  <si>
+    <t>Ha, men yomg‘irli ob-havoni juda yoqtiraman.</t>
+  </si>
+  <si>
+    <t>Yozda havo issiq bo‘ladi-mi?</t>
+  </si>
+  <si>
+    <t>Yes, it is very hot in the summer.</t>
+  </si>
+  <si>
+    <t>Ha, yozda juda issiq bo‘ladi.</t>
+  </si>
+  <si>
+    <t>Qishda havo qanday bo‘ladi?</t>
+  </si>
+  <si>
+    <t>The weather is not very good. It rarely snows.</t>
+  </si>
+  <si>
+    <t>Qishda havo unchalik yaxshi emas. Qor juda kam yog‘adi.</t>
+  </si>
+  <si>
+    <t>Yes, it is sunny today. or No, it is cloudy today.</t>
+  </si>
+  <si>
+    <t>Ha, bugun quyoshli kun. or Yo‘q, bugun bulutli kun.</t>
+  </si>
+  <si>
+    <t>Siz tez ovqat restoranlarida ovqat yeyasizmi?</t>
+  </si>
+  <si>
+    <t>Yes, I eat at KFC.</t>
+  </si>
+  <si>
+    <t>Ha, men KFCda ovqatlanaman.</t>
+  </si>
+  <si>
+    <t>Restoranda nima buyurtma qilasiz?</t>
+  </si>
+  <si>
+    <t>I usually order a cheeseburger.</t>
+  </si>
+  <si>
+    <t>Men odatda cheeseburger buyurtma qilaman.</t>
+  </si>
+  <si>
+    <t>Kafega qilgan tashrifingizni tasvirlab bering. Nima yedingiz?</t>
+  </si>
+  <si>
+    <t>I went to a café last weekend. I ate a cheeseburger and drank cola.</t>
+  </si>
+  <si>
+    <t>O‘tgan hafta oxirida kafega bordim. Cheeseburger yedim va kola ichdim.</t>
+  </si>
+  <si>
+    <t>Restoranda nimani yeyishni yoqtirasiz?</t>
+  </si>
+  <si>
+    <t>I like eating salad and steak at restaurants.</t>
+  </si>
+  <si>
+    <t>Men restoranda salat va steyk yeyishni yoqtiraman.</t>
+  </si>
+  <si>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>Weather and Eat</t>
+  </si>
+  <si>
+    <t>Mavzular</t>
+  </si>
+  <si>
+    <t>Mavzular nomi</t>
+  </si>
+  <si>
+    <t>Qism</t>
+  </si>
+  <si>
+    <t>Sovollar</t>
+  </si>
+  <si>
+    <t>Sovollar (UZ)</t>
+  </si>
+  <si>
+    <t>Jovoblar (EN)</t>
+  </si>
+  <si>
+    <t>Jovoblar (UZ)</t>
   </si>
 </sst>
 </file>
@@ -972,1202 +1443,1883 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="42.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="42.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>341</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>92</v>
+        <v>342</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>343</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>98</v>
+        <v>344</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>252</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>0</v>
+        <v>252</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>0</v>
+        <v>252</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>0</v>
+        <v>252</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>252</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>252</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>252</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>252</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>0</v>
+        <v>251</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>0</v>
+        <v>251</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>0</v>
+        <v>251</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G12" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>0</v>
+        <v>251</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>251</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G14" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>251</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>251</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>251</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>0</v>
+        <v>246</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>0</v>
+        <v>246</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="E19" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>0</v>
+        <v>246</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>0</v>
+        <v>246</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>246</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>246</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="E23" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>6</v>
+        <v>246</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>6</v>
+        <v>246</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="E25" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>0</v>
+        <v>247</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>0</v>
+        <v>247</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>170</v>
+        <v>233</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>0</v>
+        <v>247</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>0</v>
+        <v>247</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="E29" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>6</v>
+        <v>247</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="E30" s="1" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>6</v>
+        <v>247</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="E31" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>6</v>
+        <v>247</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="E32" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>6</v>
+        <v>247</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="E33" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>0</v>
+        <v>248</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>0</v>
+        <v>248</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>0</v>
+        <v>248</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>0</v>
+        <v>248</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E37" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>6</v>
+        <v>248</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E38" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>6</v>
+        <v>248</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E39" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>6</v>
+        <v>248</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E40" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>6</v>
+        <v>248</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E41" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>0</v>
+        <v>249</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E42" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>0</v>
+        <v>249</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E43" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>0</v>
+        <v>249</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E44" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>0</v>
+        <v>249</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E45" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>6</v>
+        <v>249</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E46" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>6</v>
+        <v>249</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E47" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>6</v>
+        <v>249</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E48" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>6</v>
+        <v>249</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="E49" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="E50" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E51" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>240</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E53" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>6</v>
+        <v>250</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="E54" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>6</v>
+        <v>250</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="E55" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>6</v>
+        <v>250</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="E56" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>6</v>
+        <v>250</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E57" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>0</v>
+        <v>289</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E58" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>0</v>
+        <v>289</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E59" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>0</v>
+        <v>289</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E60" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>0</v>
+        <v>289</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E61" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>6</v>
+        <v>289</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="E62" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>6</v>
+        <v>289</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E63" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>6</v>
+        <v>289</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E64" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>6</v>
+        <v>289</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E65" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E66" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E67" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E68" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E69" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E70" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E71" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E72" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
       <c r="C73" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E73" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>0</v>
+        <v>339</v>
       </c>
       <c r="C74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E74" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>0</v>
+        <v>339</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E75" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>0</v>
+        <v>339</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E76" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>0</v>
+        <v>339</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E77" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>6</v>
+        <v>339</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E78" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>6</v>
+        <v>339</v>
       </c>
       <c r="C79" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="E79" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>6</v>
+        <v>339</v>
       </c>
       <c r="C80" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E80" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>6</v>
+        <v>339</v>
       </c>
       <c r="C81" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>91</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final aggressive compact layout fix v5
</commit_message>
<xml_diff>
--- a/exam.xlsx
+++ b/exam.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e.bilolov\Desktop\Visual Studio\exam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\OneDrive\Рабочий стол\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C34CAD-51B6-4C9C-B1E1-01E6A02BCB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14415" yWindow="30" windowWidth="14340" windowHeight="17265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8784"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="352">
   <si>
     <t>Part 1</t>
   </si>
@@ -322,16 +321,6 @@
   </si>
   <si>
     <t>Sening mamlakatingda kiyimlar arzonmi?</t>
-  </si>
-  <si>
-    <t>Yes, I like shopping.
-I like buying new clothes.
-Shopping is fun.</t>
-  </si>
-  <si>
-    <t>Ha, men xarid qilishni yoqtiraman.
-Men yangi kiyimlar sotib olishni yaxshi ko‘raman.
-Xarid qilish qiziqarli.</t>
   </si>
   <si>
     <t>Yes, I go shopping on Sundays.
@@ -1113,22 +1102,47 @@
     <t>Qism</t>
   </si>
   <si>
-    <t>Sovollar</t>
-  </si>
-  <si>
-    <t>Sovollar (UZ)</t>
-  </si>
-  <si>
-    <t>Jovoblar (EN)</t>
-  </si>
-  <si>
-    <t>Jovoblar (UZ)</t>
+    <t>" What do you do in your free time?
+*Full Answer* In my free time I play video games.
+*Reason* Because I am tired after the lesson
+*Example* For example, after Inter Nation I go home or go out with my friends to play online games
+*Extra information* And also in my free time I do my homework or watch TV."</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Questions (UZ)</t>
+  </si>
+  <si>
+    <t>Full Answer (EN)</t>
+  </si>
+  <si>
+    <t>Full Answer (UZ)</t>
+  </si>
+  <si>
+    <t>Reason (EN)</t>
+  </si>
+  <si>
+    <t>Reason (UZ)</t>
+  </si>
+  <si>
+    <t>Example (UZ)</t>
+  </si>
+  <si>
+    <t>Example (EN)</t>
+  </si>
+  <si>
+    <t>Extra information (EN)</t>
+  </si>
+  <si>
+    <t>Extra information (UZ)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1442,1884 +1456,1909 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:M2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="42.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="37.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="25.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.44140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.21875" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="141.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>154</v>
+        <v>106</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E26" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>233</v>
+        <v>160</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>167</v>
+        <v>231</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E34" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E42" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E50" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E52" t="s">
-        <v>240</v>
+        <v>58</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>235</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>243</v>
+        <v>59</v>
+      </c>
+      <c r="E53" t="s">
+        <v>238</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E58" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="F57" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D65" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E66" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D73" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E74" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G74" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="F73" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D81" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E82" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="G82" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>